<commit_message>
update export template author
</commit_message>
<xml_diff>
--- a/src/main/resources/report/author_report.xlsx
+++ b/src/main/resources/report/author_report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -35,7 +35,7 @@
             <charset val="1"/>
           </rPr>
           <t>Author:
-jx:area(lastCell="C1")</t>
+jx:area(lastCell="C2")</t>
         </r>
         <r>
           <rPr>
@@ -45,7 +45,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="data" var="r" lastCell="C1")</t>
+jx:each(items="data" var="r" lastCell="C2")</t>
         </r>
       </text>
     </comment>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>${r.id}</t>
   </si>
@@ -63,13 +63,22 @@
   </si>
   <si>
     <t>${r.address}</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +98,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,8 +133,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,28 +421,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="1" max="2" width="8.7265625" style="2"/>
+    <col min="3" max="3" width="24.26953125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>